<commit_message>
no msg this time
</commit_message>
<xml_diff>
--- a/SDGT/masterGTlist.xlsx
+++ b/SDGT/masterGTlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="10760" yWindow="160" windowWidth="15360" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>1-&gt;2</t>
   </si>
@@ -43,6 +43,150 @@
   </si>
   <si>
     <t>B+</t>
+  </si>
+  <si>
+    <t>18O</t>
+  </si>
+  <si>
+    <t>18F</t>
+  </si>
+  <si>
+    <t>19O</t>
+  </si>
+  <si>
+    <t>19F</t>
+  </si>
+  <si>
+    <t>20O</t>
+  </si>
+  <si>
+    <t>20F</t>
+  </si>
+  <si>
+    <t>21O</t>
+  </si>
+  <si>
+    <t>21F</t>
+  </si>
+  <si>
+    <t>22O</t>
+  </si>
+  <si>
+    <t>22F</t>
+  </si>
+  <si>
+    <t>23O</t>
+  </si>
+  <si>
+    <t>23F</t>
+  </si>
+  <si>
+    <t>24O</t>
+  </si>
+  <si>
+    <t>24F</t>
+  </si>
+  <si>
+    <t>25O</t>
+  </si>
+  <si>
+    <t>25F</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>18Ne</t>
+  </si>
+  <si>
+    <t>19Ne</t>
+  </si>
+  <si>
+    <t>20Ne</t>
+  </si>
+  <si>
+    <t>21Ne</t>
+  </si>
+  <si>
+    <t>22Ne</t>
+  </si>
+  <si>
+    <t>23Ne</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>24Ne</t>
+  </si>
+  <si>
+    <t>25Ne</t>
+  </si>
+  <si>
+    <t>26F</t>
+  </si>
+  <si>
+    <t>26Ne</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>19Na</t>
+  </si>
+  <si>
+    <t>20Na</t>
+  </si>
+  <si>
+    <t>21Na</t>
+  </si>
+  <si>
+    <t>22Na</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23Na</t>
+  </si>
+  <si>
+    <t>24Na</t>
+  </si>
+  <si>
+    <t>25Na</t>
+  </si>
+  <si>
+    <t>26Na</t>
+  </si>
+  <si>
+    <t>20Mg</t>
+  </si>
+  <si>
+    <t>21Mg</t>
+  </si>
+  <si>
+    <t>22Mg</t>
+  </si>
+  <si>
+    <t>23Na</t>
+  </si>
+  <si>
+    <t>23Mg</t>
+  </si>
+  <si>
+    <t>24Mg</t>
+  </si>
+  <si>
+    <t>25Mg</t>
+  </si>
+  <si>
+    <t>26Mg</t>
+  </si>
+  <si>
+    <t>27Na</t>
+  </si>
+  <si>
+    <t>27Mg</t>
   </si>
 </sst>
 </file>
@@ -411,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F4"/>
+  <dimension ref="A3:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -450,7 +594,451 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete O and F
</commit_message>
<xml_diff>
--- a/SDGT/masterGTlist.xlsx
+++ b/SDGT/masterGTlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="233">
   <si>
     <t>1-&gt;2</t>
   </si>
@@ -387,22 +387,13 @@
     <t>27Ar</t>
   </si>
   <si>
-    <t>18F-&gt;18O</t>
-  </si>
-  <si>
     <t>18O-&gt;18F</t>
   </si>
   <si>
     <t>19F-&gt;19Ne</t>
   </si>
   <si>
-    <t>21Mg-&gt;21Na</t>
-  </si>
-  <si>
     <t>21Na-&gt;21Mg</t>
-  </si>
-  <si>
-    <t>24P-&gt;24Si</t>
   </si>
   <si>
     <t>24Si-&gt;24P</t>
@@ -1098,7 +1089,7 @@
   <dimension ref="A3:H149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1116,10 +1107,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1349,7 +1340,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -1360,6 +1351,9 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
@@ -1369,16 +1363,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
@@ -1389,16 +1386,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C15">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
@@ -1421,10 +1421,13 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
         <v>122</v>
       </c>
-      <c r="F17" t="s">
-        <v>123</v>
+      <c r="G17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1441,7 +1444,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
@@ -1481,10 +1484,10 @@
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
         <v>25</v>
@@ -1541,10 +1544,10 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1578,40 +1581,49 @@
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>233</v>
+        <v>230</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C27">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>234</v>
+        <v>231</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C28">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>235</v>
+        <v>232</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1628,10 +1640,10 @@
         <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1645,10 +1657,10 @@
         <v>38</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1679,10 +1691,10 @@
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F33" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1767,10 +1779,10 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1818,7 +1830,7 @@
         <v>49</v>
       </c>
       <c r="E42" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F42" t="s">
         <v>7</v>
@@ -1886,15 +1898,15 @@
         <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C47">
         <v>9</v>
@@ -1903,15 +1915,15 @@
         <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F47" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C48">
         <v>10</v>
@@ -1920,10 +1932,10 @@
         <v>64</v>
       </c>
       <c r="E48" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F48" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1974,10 +1986,10 @@
         <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F52" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1991,10 +2003,10 @@
         <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2011,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2130,10 +2142,10 @@
         <v>69</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F62" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2147,7 +2159,7 @@
         <v>70</v>
       </c>
       <c r="E63" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F63" t="s">
         <v>7</v>
@@ -2164,10 +2176,10 @@
         <v>71</v>
       </c>
       <c r="E64" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F64" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2181,10 +2193,10 @@
         <v>72</v>
       </c>
       <c r="E65" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F65" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2198,7 +2210,7 @@
         <v>73</v>
       </c>
       <c r="E66" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F66" t="s">
         <v>7</v>
@@ -2266,10 +2278,10 @@
         <v>78</v>
       </c>
       <c r="E70" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F70" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2283,10 +2295,10 @@
         <v>80</v>
       </c>
       <c r="E71" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F71" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2303,7 +2315,7 @@
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2320,10 +2332,10 @@
         <v>83</v>
       </c>
       <c r="E74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F74" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2354,10 +2366,10 @@
         <v>85</v>
       </c>
       <c r="E76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F76" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2371,10 +2383,10 @@
         <v>86</v>
       </c>
       <c r="E77" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F77" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2388,10 +2400,10 @@
         <v>87</v>
       </c>
       <c r="E78" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F78" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2405,10 +2417,10 @@
         <v>88</v>
       </c>
       <c r="E79" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F79" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2425,7 +2437,7 @@
         <v>6</v>
       </c>
       <c r="F80" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2439,10 +2451,10 @@
         <v>90</v>
       </c>
       <c r="E81" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F81" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2456,10 +2468,10 @@
         <v>91</v>
       </c>
       <c r="E82" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F82" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2544,10 +2556,10 @@
         <v>97</v>
       </c>
       <c r="E88" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F88" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2561,10 +2573,10 @@
         <v>98</v>
       </c>
       <c r="E89" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F89" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2595,10 +2607,10 @@
         <v>101</v>
       </c>
       <c r="E91" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F91" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2612,10 +2624,10 @@
         <v>100</v>
       </c>
       <c r="E92" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F92" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2649,7 +2661,7 @@
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2717,7 +2729,7 @@
         <v>6</v>
       </c>
       <c r="F98" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3010,7 +3022,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C122">
         <v>11</v>
@@ -3018,7 +3030,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C123">
         <v>12</v>
@@ -3041,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E125" t="s">
         <v>6</v>
@@ -3052,7 +3064,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C126">
         <v>2</v>
@@ -3066,7 +3078,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C127">
         <v>3</v>
@@ -3080,7 +3092,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C128">
         <v>4</v>
@@ -3094,7 +3106,7 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C129">
         <v>5</v>
@@ -3108,7 +3120,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C130">
         <v>6</v>
@@ -3122,7 +3134,7 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C131">
         <v>7</v>
@@ -3136,35 +3148,35 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C132">
         <v>8</v>
       </c>
       <c r="E132" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F132" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C133">
         <v>9</v>
       </c>
       <c r="E133" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F133" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C134">
         <v>10</v>
@@ -3178,35 +3190,35 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C135">
         <v>11</v>
       </c>
       <c r="E135" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F135" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C136">
         <v>12</v>
       </c>
       <c r="E136" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F136" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B138">
         <v>11</v>
@@ -3215,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E138" t="s">
         <v>6</v>
@@ -3226,7 +3238,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C139">
         <v>2</v>
@@ -3240,7 +3252,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -3254,7 +3266,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C141">
         <v>4</v>
@@ -3268,7 +3280,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C142">
         <v>5</v>
@@ -3282,49 +3294,49 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C143">
         <v>6</v>
       </c>
       <c r="E143" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F143" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C144">
         <v>7</v>
       </c>
       <c r="E144" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F144" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C145">
         <v>8</v>
       </c>
       <c r="E145" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F145" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C146">
         <v>9</v>
@@ -3338,7 +3350,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C147">
         <v>10</v>
@@ -3352,7 +3364,7 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C148">
         <v>11</v>
@@ -3366,13 +3378,13 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C149">
         <v>12</v>
       </c>
       <c r="D149" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now up through Ne
</commit_message>
<xml_diff>
--- a/SDGT/masterGTlist.xlsx
+++ b/SDGT/masterGTlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="0" windowWidth="25600" windowHeight="16160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="228">
   <si>
     <t>1-&gt;2</t>
   </si>
@@ -402,24 +402,12 @@
     <t>37Cl</t>
   </si>
   <si>
-    <t>26S-&gt;26Cl</t>
-  </si>
-  <si>
-    <t>19F-&gt;19O</t>
-  </si>
-  <si>
     <t>19O-&gt;19F</t>
   </si>
   <si>
-    <t>20Ne-&gt;20F</t>
-  </si>
-  <si>
     <t>20F-&gt;20Ne</t>
   </si>
   <si>
-    <t>22Mg-&gt;22Na</t>
-  </si>
-  <si>
     <t>22Na-&gt;22Mg</t>
   </si>
   <si>
@@ -706,6 +694,15 @@
   </si>
   <si>
     <t>29Ne</t>
+  </si>
+  <si>
+    <t>30Ne</t>
+  </si>
+  <si>
+    <t>30Na</t>
+  </si>
+  <si>
+    <t>na/</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H149"/>
+  <dimension ref="A3:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1328,7 +1325,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -1351,13 +1348,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -1374,13 +1371,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C15">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -1417,6 +1414,9 @@
       <c r="G17" t="s">
         <v>32</v>
       </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
@@ -1437,6 +1437,9 @@
       <c r="G18" t="s">
         <v>32</v>
       </c>
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
@@ -1569,49 +1572,58 @@
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C27">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C28">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1628,10 +1640,13 @@
         <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1645,10 +1660,13 @@
         <v>38</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1667,8 +1685,14 @@
       <c r="F32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1679,13 +1703,16 @@
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>129</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1701,8 +1728,11 @@
       <c r="F34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1718,8 +1748,14 @@
       <c r="F35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1735,8 +1771,14 @@
       <c r="F36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" t="s">
+        <v>227</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1752,277 +1794,271 @@
       <c r="F37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="C38">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B43">
         <v>3</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <v>1</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D43" t="s">
         <v>45</v>
       </c>
-      <c r="E39" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="E43" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="C40">
+      <c r="C44">
         <v>2</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D44" t="s">
         <v>46</v>
       </c>
-      <c r="E40" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="C41">
+      <c r="C45">
         <v>3</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D45" t="s">
         <v>47</v>
       </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="C42">
+      <c r="C46">
         <v>4</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D46" t="s">
         <v>49</v>
       </c>
-      <c r="E42" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
+      <c r="E46" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="C47">
         <v>5</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D47" t="s">
         <v>50</v>
       </c>
-      <c r="E43" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
         <v>43</v>
       </c>
-      <c r="C44">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
         <v>51</v>
       </c>
-      <c r="E44" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
         <v>44</v>
       </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
         <v>52</v>
       </c>
-      <c r="E45" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>54</v>
-      </c>
-      <c r="E46" t="s">
-        <v>137</v>
-      </c>
-      <c r="F46" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>164</v>
-      </c>
-      <c r="C47">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E47" t="s">
-        <v>200</v>
-      </c>
-      <c r="F47" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>64</v>
-      </c>
-      <c r="E48" t="s">
-        <v>202</v>
-      </c>
-      <c r="F48" t="s">
-        <v>203</v>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="F50" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>160</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="F51" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E52" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="F52" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>58</v>
-      </c>
-      <c r="E53" t="s">
-        <v>198</v>
-      </c>
-      <c r="F53" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>166</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E55" t="s">
         <v>6</v>
@@ -2033,84 +2069,98 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="F56" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="F57" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E58" t="s">
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
         <v>6</v>
       </c>
       <c r="F59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -2121,101 +2171,87 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>167</v>
+        <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>168</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
-        <v>173</v>
+        <v>6</v>
       </c>
       <c r="F63" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
-      </c>
-      <c r="D64" t="s">
-        <v>71</v>
-      </c>
-      <c r="E64" t="s">
-        <v>174</v>
-      </c>
-      <c r="F64" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E65" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C66">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E66" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="F66" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C67">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E67" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="F67" t="s">
         <v>7</v>
@@ -2223,308 +2259,322 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C68">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E68" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="F68" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C69">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E69" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C70">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F70" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C71">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E71" t="s">
-        <v>209</v>
+        <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>210</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C72">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E72" t="s">
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>193</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>69</v>
-      </c>
-      <c r="B74">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E74" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="F74" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D75" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E75" t="s">
-        <v>6</v>
+        <v>205</v>
       </c>
       <c r="F75" t="s">
-        <v>7</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E76" t="s">
-        <v>171</v>
+        <v>6</v>
       </c>
       <c r="F76" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77">
-        <v>4</v>
-      </c>
-      <c r="D77" t="s">
-        <v>86</v>
-      </c>
-      <c r="E77" t="s">
-        <v>178</v>
-      </c>
-      <c r="F77" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="B78">
+        <v>6</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E78" t="s">
-        <v>211</v>
+        <v>165</v>
       </c>
       <c r="F78" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C79">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C80">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E80" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="F80" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E81" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
       <c r="F81" t="s">
-        <v>217</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C82">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E82" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F82" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C83">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E83" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="F83" t="s">
-        <v>7</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C84">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E84" t="s">
         <v>6</v>
       </c>
       <c r="F84" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C85">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E85" t="s">
-        <v>6</v>
+        <v>212</v>
       </c>
       <c r="F85" t="s">
-        <v>7</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" t="s">
+        <v>214</v>
+      </c>
+      <c r="F86" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E87" t="s">
         <v>6</v>
@@ -2535,166 +2585,152 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D88" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E88" t="s">
-        <v>176</v>
+        <v>6</v>
       </c>
       <c r="F88" t="s">
-        <v>177</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C89">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E89" t="s">
-        <v>179</v>
+        <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" t="s">
-        <v>87</v>
-      </c>
-      <c r="C90">
-        <v>4</v>
-      </c>
-      <c r="D90" t="s">
-        <v>99</v>
-      </c>
-      <c r="E90" t="s">
-        <v>6</v>
-      </c>
-      <c r="F90" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="B91">
+        <v>7</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E91" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="F91" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C92">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E92" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F92" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C93">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E93" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="F93" t="s">
-        <v>7</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C94">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E94" t="s">
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C95">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="F95" t="s">
-        <v>7</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C96">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E96" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="F96" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C97">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E97" t="s">
         <v>6</v>
@@ -2705,44 +2741,64 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C98">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D98" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E98" t="s">
         <v>6</v>
       </c>
       <c r="F98" t="s">
-        <v>185</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>104</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+      <c r="F99" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>97</v>
-      </c>
-      <c r="B100">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D100" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="E100" t="s">
+        <v>6</v>
+      </c>
+      <c r="F100" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C101">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D101" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E101" t="s">
         <v>6</v>
@@ -2753,69 +2809,61 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D102" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E102" t="s">
         <v>6</v>
       </c>
       <c r="F102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" t="s">
-        <v>101</v>
-      </c>
-      <c r="C103">
-        <v>4</v>
-      </c>
-      <c r="D103" t="s">
-        <v>112</v>
-      </c>
-      <c r="E103" t="s">
-        <v>6</v>
-      </c>
-      <c r="F103" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B104">
+        <v>8</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C105">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="E105" t="s">
+        <v>6</v>
+      </c>
+      <c r="F105" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C106">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E106" t="s">
         <v>6</v>
@@ -2826,78 +2874,80 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D107" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="E107" t="s">
+        <v>6</v>
+      </c>
+      <c r="F107" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C108">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>117</v>
-      </c>
-      <c r="F108" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C109">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>118</v>
-      </c>
-      <c r="E109" t="s">
-        <v>6</v>
-      </c>
-      <c r="F109" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C110">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D110" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E110" t="s">
         <v>6</v>
       </c>
       <c r="F110" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>104</v>
+      </c>
+      <c r="C111">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>110</v>
-      </c>
-      <c r="B112">
+        <v>105</v>
+      </c>
+      <c r="C112">
         <v>9</v>
       </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
       <c r="D112" t="s">
-        <v>120</v>
-      </c>
-      <c r="E112" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="F112" t="s">
         <v>7</v>
@@ -2905,13 +2955,13 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D113" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E113" t="s">
         <v>6</v>
@@ -2922,38 +2972,36 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D114" t="s">
+        <v>119</v>
       </c>
       <c r="E114" t="s">
         <v>6</v>
       </c>
       <c r="F114" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" t="s">
-        <v>113</v>
-      </c>
-      <c r="C115">
-        <v>4</v>
-      </c>
-      <c r="E115" t="s">
-        <v>6</v>
-      </c>
-      <c r="F115" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="B116">
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>120</v>
+      </c>
+      <c r="E116" t="s">
+        <v>6</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
@@ -2961,10 +3009,13 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C117">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>121</v>
       </c>
       <c r="E117" t="s">
         <v>6</v>
@@ -2975,34 +3026,52 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C119">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="E119" t="s">
+        <v>6</v>
+      </c>
+      <c r="F119" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C120">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="F120" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C121">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="E121" t="s">
+        <v>6</v>
       </c>
       <c r="F121" t="s">
         <v>7</v>
@@ -3010,41 +3079,34 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C122">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C123">
-        <v>12</v>
-      </c>
-      <c r="E123" t="s">
-        <v>6</v>
-      </c>
-      <c r="F123" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" t="s">
+        <v>118</v>
+      </c>
+      <c r="C124">
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>121</v>
-      </c>
-      <c r="B125">
+        <v>119</v>
+      </c>
+      <c r="C125">
         <v>10</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
-      </c>
-      <c r="D125" t="s">
-        <v>124</v>
-      </c>
-      <c r="E125" t="s">
-        <v>6</v>
       </c>
       <c r="F125" t="s">
         <v>7</v>
@@ -3052,52 +3114,38 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C126">
-        <v>2</v>
-      </c>
-      <c r="E126" t="s">
-        <v>6</v>
-      </c>
-      <c r="F126" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C127">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E127" t="s">
         <v>6</v>
       </c>
       <c r="F127" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" t="s">
-        <v>141</v>
-      </c>
-      <c r="C128">
-        <v>4</v>
-      </c>
-      <c r="E128" t="s">
-        <v>6</v>
-      </c>
-      <c r="F128" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>121</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
       </c>
       <c r="C129">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
+        <v>124</v>
       </c>
       <c r="E129" t="s">
         <v>6</v>
@@ -3108,10 +3156,10 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C130">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E130" t="s">
         <v>6</v>
@@ -3122,10 +3170,10 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C131">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E131" t="s">
         <v>6</v>
@@ -3136,38 +3184,38 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C132">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E132" t="s">
-        <v>186</v>
+        <v>6</v>
       </c>
       <c r="F132" t="s">
-        <v>187</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C133">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E133" t="s">
-        <v>188</v>
+        <v>6</v>
       </c>
       <c r="F133" t="s">
-        <v>189</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C134">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E134" t="s">
         <v>6</v>
@@ -3178,44 +3226,52 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C135">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E135" t="s">
-        <v>190</v>
+        <v>6</v>
       </c>
       <c r="F135" t="s">
-        <v>190</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C136">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E136" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F136" t="s">
-        <v>192</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>142</v>
+      </c>
+      <c r="C137">
+        <v>9</v>
+      </c>
+      <c r="E137" t="s">
+        <v>184</v>
+      </c>
+      <c r="F137" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>150</v>
-      </c>
-      <c r="B138">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C138">
-        <v>1</v>
-      </c>
-      <c r="D138" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="E138" t="s">
         <v>6</v>
@@ -3226,52 +3282,44 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E139" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="F139" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C140">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E140" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="F140" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" t="s">
-        <v>155</v>
-      </c>
-      <c r="C141">
-        <v>4</v>
-      </c>
-      <c r="E141" t="s">
-        <v>6</v>
-      </c>
-      <c r="F141" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>156</v>
+        <v>146</v>
+      </c>
+      <c r="B142">
+        <v>11</v>
       </c>
       <c r="C142">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D142" t="s">
+        <v>147</v>
       </c>
       <c r="E142" t="s">
         <v>6</v>
@@ -3282,52 +3330,52 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C143">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E143" t="s">
-        <v>193</v>
+        <v>6</v>
       </c>
       <c r="F143" t="s">
-        <v>194</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C144">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E144" t="s">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="F144" t="s">
-        <v>196</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C145">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E145" t="s">
-        <v>193</v>
+        <v>6</v>
       </c>
       <c r="F145" t="s">
-        <v>197</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C146">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E146" t="s">
         <v>6</v>
@@ -3338,41 +3386,97 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C147">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E147" t="s">
-        <v>6</v>
+        <v>189</v>
       </c>
       <c r="F147" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C148">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E148" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="F148" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C149">
+        <v>8</v>
+      </c>
+      <c r="E149" t="s">
+        <v>189</v>
+      </c>
+      <c r="F149" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>156</v>
+      </c>
+      <c r="C150">
+        <v>9</v>
+      </c>
+      <c r="E150" t="s">
+        <v>6</v>
+      </c>
+      <c r="F150" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>157</v>
+      </c>
+      <c r="C151">
+        <v>10</v>
+      </c>
+      <c r="E151" t="s">
+        <v>6</v>
+      </c>
+      <c r="F151" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>158</v>
+      </c>
+      <c r="C152">
+        <v>11</v>
+      </c>
+      <c r="E152" t="s">
+        <v>6</v>
+      </c>
+      <c r="F152" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>159</v>
+      </c>
+      <c r="C153">
         <v>12</v>
       </c>
-      <c r="D149" t="s">
-        <v>153</v>
+      <c r="D153" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>